<commit_message>
new file:   final/Bayesiano/z633_lght_bin_BO_under_10repeat_v4.r 	new file:   final/Bayesiano/z633_lightgbm_binaria_BO_undersampling_v4.r 	new file:   final/FeatureEng/z815_FE_final.r 	new file:   final/FeatureEng/z815_FE_final_20220929.r 	new file:   final/z844_lightgbm_final_semillerio.r
</commit_message>
<xml_diff>
--- a/src/lightgbm/Pruebas/Simple/hiperBO.xlsx
+++ b/src/lightgbm/Pruebas/Simple/hiperBO.xlsx
@@ -479,6 +479,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -496,12 +497,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -538,12 +545,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -556,6 +571,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -567,7 +642,7 @@
   <dimension ref="A1:X121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z10" activeCellId="0" sqref="Z10"/>
+      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12:V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,21 +650,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="8.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="7.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="23" style="0" width="11.52"/>
@@ -1393,34 +1468,34 @@
       <c r="L12" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M12" s="2" t="n">
         <v>1531</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>999983</v>
-      </c>
-      <c r="P12" s="0" t="n">
+      <c r="N12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>999983</v>
+      </c>
+      <c r="P12" s="2" t="n">
         <v>0.0102532958995188</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q12" s="2" t="n">
         <v>0.229763939138759</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="R12" s="2" t="n">
         <v>7093</v>
       </c>
-      <c r="S12" s="0" t="n">
+      <c r="S12" s="2" t="n">
         <v>285</v>
       </c>
-      <c r="T12" s="0" t="n">
+      <c r="T12" s="2" t="n">
         <v>0.020169638283811</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U12" s="2" t="n">
         <v>25740000</v>
       </c>
-      <c r="V12" s="0" t="n">
+      <c r="V12" s="2" t="n">
         <v>84</v>
       </c>
     </row>

</xml_diff>